<commit_message>
30 regions. fail cal 1990 cent asia dist heat fail solve 2065
</commit_message>
<xml_diff>
--- a/gcam-data-system/energy-data/assumptions/Tables_A20s.xlsx
+++ b/gcam-data-system/energy-data/assumptions/Tables_A20s.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32140" windowHeight="21340" tabRatio="684" firstSheet="43" activeTab="43"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="684" firstSheet="26" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="A21.sector.csv" sheetId="5" r:id="rId1"/>
@@ -756,8 +756,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1685">
+  <cellStyleXfs count="1699">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2451,7 +2465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1685">
+  <cellStyles count="1699">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3294,6 +3308,13 @@
     <cellStyle name="Followed Hyperlink" xfId="1680" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1682" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1698" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4136,6 +4157,13 @@
     <cellStyle name="Hyperlink" xfId="1679" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1681" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1697" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9355,7 +9383,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10228,8 +10256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10600,7 +10628,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D17" activeCellId="1" sqref="D15 D17"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17556,7 +17584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
interpolation rules for refining sector
</commit_message>
<xml_diff>
--- a/gcam-data-system/energy-data/assumptions/Tables_A20s.xlsx
+++ b/gcam-data-system/energy-data/assumptions/Tables_A20s.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="684" firstSheet="26" activeTab="27"/>
+    <workbookView xWindow="22720" yWindow="1240" windowWidth="24980" windowHeight="16240" tabRatio="684" firstSheet="14" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="A21.sector.csv" sheetId="5" r:id="rId1"/>
@@ -22,47 +22,48 @@
     <sheet name="A22.subsector_logit.csv" sheetId="25" r:id="rId13"/>
     <sheet name="A22.subsector_shrwt.csv" sheetId="8" r:id="rId14"/>
     <sheet name="A22.subsector_interp.csv" sheetId="26" r:id="rId15"/>
-    <sheet name="A22.globaltech_cost.csv" sheetId="27" r:id="rId16"/>
-    <sheet name="A22.globaltech_coef.csv" sheetId="3" r:id="rId17"/>
-    <sheet name="A22.globaltech_shrwt.csv" sheetId="29" r:id="rId18"/>
-    <sheet name="A22.globaltech_retirement.csv" sheetId="28" r:id="rId19"/>
-    <sheet name="A22.globaltech_co2capture.csv" sheetId="30" r:id="rId20"/>
-    <sheet name="A23.sector.csv" sheetId="35" r:id="rId21"/>
-    <sheet name="A23.subsector_logit.csv" sheetId="37" r:id="rId22"/>
-    <sheet name="A23.subsector_shrwt.csv" sheetId="38" r:id="rId23"/>
-    <sheet name="A23.subsector_interp.csv" sheetId="39" r:id="rId24"/>
-    <sheet name="A23.chp_elecratio.csv" sheetId="42" r:id="rId25"/>
-    <sheet name="A23.globalinttech.csv" sheetId="49" r:id="rId26"/>
-    <sheet name="A23.globaltech_shrwt.csv" sheetId="45" r:id="rId27"/>
-    <sheet name="A23.globaltech_keyword.csv" sheetId="69" r:id="rId28"/>
-    <sheet name="A23.globaltech_eff.csv" sheetId="43" r:id="rId29"/>
-    <sheet name="A23.globaltech_capital.csv" sheetId="46" r:id="rId30"/>
-    <sheet name="A23.globaltech_OMfixed.csv" sheetId="47" r:id="rId31"/>
-    <sheet name="A23.globaltech_OMvar.csv" sheetId="44" r:id="rId32"/>
-    <sheet name="A23.globaltech_retirement.csv" sheetId="48" r:id="rId33"/>
-    <sheet name="A23.globaltech_co2capture.csv" sheetId="50" r:id="rId34"/>
-    <sheet name="A24.sector.csv" sheetId="53" r:id="rId35"/>
-    <sheet name="A24.subsector_logit.csv" sheetId="54" r:id="rId36"/>
-    <sheet name="A24.subsector_shrwt.csv" sheetId="55" r:id="rId37"/>
-    <sheet name="A24.subsector_interp.csv" sheetId="56" r:id="rId38"/>
-    <sheet name="A24.globaltech_cost.csv" sheetId="57" r:id="rId39"/>
-    <sheet name="A24.globaltech_coef.csv" sheetId="58" r:id="rId40"/>
-    <sheet name="A24.globaltech_shrwt.csv" sheetId="59" r:id="rId41"/>
-    <sheet name="A25.sector.csv" sheetId="60" r:id="rId42"/>
-    <sheet name="A25.subsector_logit.csv" sheetId="61" r:id="rId43"/>
-    <sheet name="A25.globaltech_keyword.csv" sheetId="71" r:id="rId44"/>
-    <sheet name="A25.subsector_shrwt.csv" sheetId="62" r:id="rId45"/>
-    <sheet name="A25.globaltech_cost.csv" sheetId="64" r:id="rId46"/>
-    <sheet name="A25.globaltech_eff.csv" sheetId="65" r:id="rId47"/>
-    <sheet name="A25.globaltech_shrwt.csv" sheetId="66" r:id="rId48"/>
-    <sheet name="A25.globaltech_co2capture.csv" sheetId="67" r:id="rId49"/>
-    <sheet name="A26.sector.csv" sheetId="6" r:id="rId50"/>
-    <sheet name="A26.subsector_logit.csv" sheetId="32" r:id="rId51"/>
-    <sheet name="A26.subsector_shrwt.csv" sheetId="33" r:id="rId52"/>
-    <sheet name="A26.subsector_interp.csv" sheetId="51" r:id="rId53"/>
-    <sheet name="A26.globaltech_cost.csv" sheetId="31" r:id="rId54"/>
-    <sheet name="A26.globaltech_eff.csv" sheetId="7" r:id="rId55"/>
-    <sheet name="A26.globaltech_shrwt.csv" sheetId="52" r:id="rId56"/>
+    <sheet name="A22.globaltech_interp.csv" sheetId="72" r:id="rId16"/>
+    <sheet name="A22.globaltech_cost.csv" sheetId="27" r:id="rId17"/>
+    <sheet name="A22.globaltech_coef.csv" sheetId="3" r:id="rId18"/>
+    <sheet name="A22.globaltech_shrwt.csv" sheetId="29" r:id="rId19"/>
+    <sheet name="A22.globaltech_retirement.csv" sheetId="28" r:id="rId20"/>
+    <sheet name="A22.globaltech_co2capture.csv" sheetId="30" r:id="rId21"/>
+    <sheet name="A23.sector.csv" sheetId="35" r:id="rId22"/>
+    <sheet name="A23.subsector_logit.csv" sheetId="37" r:id="rId23"/>
+    <sheet name="A23.subsector_shrwt.csv" sheetId="38" r:id="rId24"/>
+    <sheet name="A23.subsector_interp.csv" sheetId="39" r:id="rId25"/>
+    <sheet name="A23.chp_elecratio.csv" sheetId="42" r:id="rId26"/>
+    <sheet name="A23.globalinttech.csv" sheetId="49" r:id="rId27"/>
+    <sheet name="A23.globaltech_shrwt.csv" sheetId="45" r:id="rId28"/>
+    <sheet name="A23.globaltech_keyword.csv" sheetId="69" r:id="rId29"/>
+    <sheet name="A23.globaltech_eff.csv" sheetId="43" r:id="rId30"/>
+    <sheet name="A23.globaltech_capital.csv" sheetId="46" r:id="rId31"/>
+    <sheet name="A23.globaltech_OMfixed.csv" sheetId="47" r:id="rId32"/>
+    <sheet name="A23.globaltech_OMvar.csv" sheetId="44" r:id="rId33"/>
+    <sheet name="A23.globaltech_retirement.csv" sheetId="48" r:id="rId34"/>
+    <sheet name="A23.globaltech_co2capture.csv" sheetId="50" r:id="rId35"/>
+    <sheet name="A24.sector.csv" sheetId="53" r:id="rId36"/>
+    <sheet name="A24.subsector_logit.csv" sheetId="54" r:id="rId37"/>
+    <sheet name="A24.subsector_shrwt.csv" sheetId="55" r:id="rId38"/>
+    <sheet name="A24.subsector_interp.csv" sheetId="56" r:id="rId39"/>
+    <sheet name="A24.globaltech_cost.csv" sheetId="57" r:id="rId40"/>
+    <sheet name="A24.globaltech_coef.csv" sheetId="58" r:id="rId41"/>
+    <sheet name="A24.globaltech_shrwt.csv" sheetId="59" r:id="rId42"/>
+    <sheet name="A25.sector.csv" sheetId="60" r:id="rId43"/>
+    <sheet name="A25.subsector_logit.csv" sheetId="61" r:id="rId44"/>
+    <sheet name="A25.globaltech_keyword.csv" sheetId="71" r:id="rId45"/>
+    <sheet name="A25.subsector_shrwt.csv" sheetId="62" r:id="rId46"/>
+    <sheet name="A25.globaltech_cost.csv" sheetId="64" r:id="rId47"/>
+    <sheet name="A25.globaltech_eff.csv" sheetId="65" r:id="rId48"/>
+    <sheet name="A25.globaltech_shrwt.csv" sheetId="66" r:id="rId49"/>
+    <sheet name="A25.globaltech_co2capture.csv" sheetId="67" r:id="rId50"/>
+    <sheet name="A26.sector.csv" sheetId="6" r:id="rId51"/>
+    <sheet name="A26.subsector_logit.csv" sheetId="32" r:id="rId52"/>
+    <sheet name="A26.subsector_shrwt.csv" sheetId="33" r:id="rId53"/>
+    <sheet name="A26.subsector_interp.csv" sheetId="51" r:id="rId54"/>
+    <sheet name="A26.globaltech_cost.csv" sheetId="31" r:id="rId55"/>
+    <sheet name="A26.globaltech_eff.csv" sheetId="7" r:id="rId56"/>
+    <sheet name="A26.globaltech_shrwt.csv" sheetId="52" r:id="rId57"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2583" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2624" uniqueCount="209">
   <si>
     <t>technology</t>
   </si>
@@ -699,6 +700,9 @@
   <si>
     <t># Hydrogen technology keywords</t>
   </si>
+  <si>
+    <t># Primary energy transformation technology interpolation (for techs that may have cal values in subsectors with multiple calibrated technologies)</t>
+  </si>
 </sst>
 </file>
 
@@ -756,8 +760,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1699">
+  <cellStyleXfs count="1709">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2465,7 +2479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1699">
+  <cellStyles count="1709">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3315,6 +3329,11 @@
     <cellStyle name="Followed Hyperlink" xfId="1694" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1696" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1708" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4164,6 +4183,11 @@
     <cellStyle name="Hyperlink" xfId="1693" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1695" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1707" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4496,7 +4520,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A2" sqref="A2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4729,7 +4753,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4843,7 +4867,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5031,7 +5055,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5136,7 +5160,7 @@
         <v>43</v>
       </c>
       <c r="C9">
-        <v>-13</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5147,7 +5171,7 @@
         <v>45</v>
       </c>
       <c r="C10">
-        <v>-13</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -5356,7 +5380,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C2" sqref="C2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5590,10 +5614,179 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3">
+        <v>2020</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4">
+        <v>2020</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6083,12 +6276,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6213,16 +6406,13 @@
         <v>23</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:G7" si="0">1/421.377</f>
-        <v>2.3731717677993817E-3</v>
+        <v>2.3731720000000002E-3</v>
       </c>
       <c r="F6">
-        <f>1/421.377</f>
-        <v>2.3731717677993817E-3</v>
+        <v>2.3731720000000002E-3</v>
       </c>
       <c r="G6">
-        <f>1/421.377</f>
-        <v>2.3731717677993817E-3</v>
+        <v>2.3731720000000002E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6239,16 +6429,13 @@
         <v>23</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>2.3731717677993817E-3</v>
+        <v>2.3731720000000002E-3</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>2.3731717677993817E-3</v>
+        <v>2.3731720000000002E-3</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
-        <v>2.3731717677993817E-3</v>
+        <v>2.3731720000000002E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6356,17 +6543,14 @@
       <c r="D12" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="1">
-        <f>E11*1.04</f>
-        <v>2.1964800000000002</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" ref="F12:G12" si="1">F11*1.04</f>
-        <v>2.1964800000000002</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>2.0373600000000001</v>
+      <c r="E12">
+        <v>2.1960000000000002</v>
+      </c>
+      <c r="F12">
+        <v>2.1960000000000002</v>
+      </c>
+      <c r="G12">
+        <v>2.0369999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6382,17 +6566,14 @@
       <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="1">
-        <f>E11*1.1</f>
-        <v>2.3232000000000004</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" ref="F13:G13" si="2">F11*1.1</f>
-        <v>2.3232000000000004</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" si="2"/>
-        <v>2.1549</v>
+      <c r="E13">
+        <v>2.323</v>
+      </c>
+      <c r="F13">
+        <v>2.323</v>
+      </c>
+      <c r="G13">
+        <v>2.1549999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -6454,17 +6635,14 @@
       <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="1">
-        <f>E15*1.04</f>
-        <v>2.1392799999999998</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" ref="F16" si="3">F15*1.04</f>
-        <v>2.1392799999999998</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" ref="G16" si="4">G15*1.04</f>
-        <v>1.8418399999999999</v>
+      <c r="E16">
+        <v>2.1389999999999998</v>
+      </c>
+      <c r="F16">
+        <v>2.1389999999999998</v>
+      </c>
+      <c r="G16">
+        <v>1.8420000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -6480,17 +6658,14 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="1">
-        <f>E15*1.1</f>
-        <v>2.2627000000000002</v>
-      </c>
-      <c r="F17" s="1">
-        <f t="shared" ref="F17:G17" si="5">F15*1.1</f>
-        <v>2.2627000000000002</v>
-      </c>
-      <c r="G17" s="1">
-        <f t="shared" si="5"/>
-        <v>1.9481000000000002</v>
+      <c r="E17">
+        <v>2.2629999999999999</v>
+      </c>
+      <c r="F17">
+        <v>2.2629999999999999</v>
+      </c>
+      <c r="G17">
+        <v>1.948</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -6529,17 +6704,14 @@
       <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="1">
-        <f>E18*1.04</f>
-        <v>2.0394400000000004</v>
-      </c>
-      <c r="F19" s="1">
-        <f t="shared" ref="F19" si="6">F18*1.04</f>
-        <v>2.0394400000000004</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" ref="G19" si="7">G18*1.04</f>
-        <v>1.8085600000000002</v>
+      <c r="E19">
+        <v>2.0390000000000001</v>
+      </c>
+      <c r="F19">
+        <v>2.0390000000000001</v>
+      </c>
+      <c r="G19">
+        <v>1.8089999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -6555,17 +6727,14 @@
       <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="1">
-        <f>E18*1.1</f>
-        <v>2.1571000000000002</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" ref="F20:G20" si="8">F18*1.1</f>
-        <v>2.1571000000000002</v>
-      </c>
-      <c r="G20" s="1">
-        <f t="shared" si="8"/>
-        <v>1.9129000000000003</v>
+      <c r="E20">
+        <v>2.157</v>
+      </c>
+      <c r="F20">
+        <v>2.157</v>
+      </c>
+      <c r="G20">
+        <v>1.913</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -6717,12 +6886,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7271,12 +7440,197 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>-6</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>-6</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>-6</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>-6</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>-6</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>-6</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>-3</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10">
+        <v>-6</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11">
+        <v>-6</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A2" sqref="A2:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7979,197 +8333,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>-6</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>-6</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>-6</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>-6</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>-6</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>-6</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>-3</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10">
-        <v>-6</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11">
-        <v>-6</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8315,7 +8484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -8417,7 +8586,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -8574,7 +8743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -8780,7 +8949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -9119,7 +9288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -9182,7 +9351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -9378,12 +9547,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10252,11 +10421,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -10623,7 +10792,230 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>2050</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O27"/>
   <sheetViews>
@@ -11878,230 +12270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>2050</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
@@ -13287,7 +13456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
@@ -14421,7 +14590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
@@ -15218,7 +15387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -15921,7 +16090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -16098,7 +16267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -16165,7 +16334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -16256,7 +16425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -16365,7 +16534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -16504,7 +16673,301 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>2050</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8">
+        <v>2185</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9">
+        <v>2050</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
@@ -16741,301 +17204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7">
-        <v>2050</v>
-      </c>
-      <c r="G7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8">
-        <v>2185</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9">
-        <v>2050</v>
-      </c>
-      <c r="G9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -17167,7 +17336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -17283,7 +17452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -17401,7 +17570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -17580,7 +17749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -17755,7 +17924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
@@ -18143,7 +18312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
@@ -18786,7 +18955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
@@ -19427,7 +19596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -19730,7 +19899,279 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2">
+        <v>1971</v>
+      </c>
+      <c r="F2">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="F3">
+        <v>0.73699999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4">
+        <v>0.15</v>
+      </c>
+      <c r="F4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5">
+        <v>0.25</v>
+      </c>
+      <c r="F5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6">
+        <v>0.15</v>
+      </c>
+      <c r="F6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7">
+        <v>0.15</v>
+      </c>
+      <c r="F7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -19878,279 +20319,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2">
-        <v>1971</v>
-      </c>
-      <c r="F2">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="F3">
-        <v>0.73699999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4">
-        <v>0.15</v>
-      </c>
-      <c r="F4">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5">
-        <v>0.25</v>
-      </c>
-      <c r="F5">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6">
-        <v>0.15</v>
-      </c>
-      <c r="F6">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7">
-        <v>0.15</v>
-      </c>
-      <c r="F7">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" t="s">
-        <v>185</v>
-      </c>
-      <c r="D11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" t="s">
-        <v>186</v>
-      </c>
-      <c r="D12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>187</v>
-      </c>
-      <c r="D13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -20421,7 +20590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -20611,7 +20780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -20846,7 +21015,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -21123,7 +21292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -21519,7 +21688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -21878,7 +22047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -22224,7 +22393,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -22436,14 +22605,14 @@
       <c r="D10" t="s">
         <v>183</v>
       </c>
-      <c r="E10" s="3">
-        <v>111.78730206783794</v>
-      </c>
-      <c r="F10" s="3">
-        <v>111.78730206783794</v>
-      </c>
-      <c r="G10" s="3">
-        <v>111.78730206783794</v>
+      <c r="E10">
+        <v>111.79</v>
+      </c>
+      <c r="F10">
+        <v>111.79</v>
+      </c>
+      <c r="G10">
+        <v>111.79</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -22459,14 +22628,14 @@
       <c r="D11" t="s">
         <v>184</v>
       </c>
-      <c r="E11" s="3">
-        <v>582.47719635002909</v>
-      </c>
-      <c r="F11" s="3">
-        <v>582.47719635002909</v>
-      </c>
-      <c r="G11" s="3">
-        <v>582.47719635002909</v>
+      <c r="E11">
+        <v>582.48</v>
+      </c>
+      <c r="F11">
+        <v>582.48</v>
+      </c>
+      <c r="G11">
+        <v>582.48</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -22505,14 +22674,14 @@
       <c r="D13" t="s">
         <v>186</v>
       </c>
-      <c r="E13" s="3">
-        <v>142.57460317460317</v>
-      </c>
-      <c r="F13" s="3">
-        <v>142.57460317460317</v>
-      </c>
-      <c r="G13" s="3">
-        <v>142.57460317460317</v>
+      <c r="E13">
+        <v>142.57</v>
+      </c>
+      <c r="F13">
+        <v>142.57</v>
+      </c>
+      <c r="G13">
+        <v>142.57</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -22528,13 +22697,13 @@
       <c r="D14" t="s">
         <v>187</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
         <v>128</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <v>128</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14">
         <v>128</v>
       </c>
     </row>
@@ -22625,7 +22794,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
corrected delivery costs for gas, electricity, and refined liquids
</commit_message>
<xml_diff>
--- a/gcam-data-system/energy-data/assumptions/Tables_A20s.xlsx
+++ b/gcam-data-system/energy-data/assumptions/Tables_A20s.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22720" yWindow="1240" windowWidth="24980" windowHeight="16240" tabRatio="684" firstSheet="14" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="684" firstSheet="52" activeTab="54"/>
   </bookViews>
   <sheets>
     <sheet name="A21.sector.csv" sheetId="5" r:id="rId1"/>
@@ -5616,7 +5616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -21296,8 +21296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21457,16 +21457,16 @@
         <v>57</v>
       </c>
       <c r="E7">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -21613,16 +21613,16 @@
         <v>57</v>
       </c>
       <c r="E13">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="F13">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="G13">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="H13">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -21639,16 +21639,16 @@
         <v>57</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:8">

</xml_diff>